<commit_message>
Lab 0 - 4 updates commit
</commit_message>
<xml_diff>
--- a/assignments/Lab4_Tables.xlsx
+++ b/assignments/Lab4_Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18165\Documents\R\Lab\biostatlab\assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442E5380-9811-4A7F-BEDE-12F3F0EEB284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BE50F0-C2AD-4433-97BC-C84986055965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{441DAC2A-7180-4E9D-9169-FCB49694DB4E}"/>
   </bookViews>
@@ -488,85 +488,85 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -898,7 +898,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13:J18"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -923,20 +923,20 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
       <c r="E1" s="26"/>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="48" t="s">
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="50"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="46"/>
     </row>
     <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27"/>
@@ -946,24 +946,24 @@
       <c r="E2" s="29"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
-      <c r="H2" s="53" t="s">
+      <c r="H2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="54"/>
+      <c r="I2" s="31"/>
       <c r="J2" s="23"/>
       <c r="K2" s="24"/>
       <c r="L2" s="25"/>
-      <c r="M2" s="46" t="s">
+      <c r="M2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="47"/>
+      <c r="N2" s="56"/>
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:15" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="32" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -972,63 +972,63 @@
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="51" t="s">
+      <c r="I3" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="41" t="s">
+      <c r="L3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="41" t="s">
+      <c r="M3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="41" t="s">
+      <c r="N3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="41" t="s">
+      <c r="O3" s="42" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="56"/>
-      <c r="B4" s="56"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="56"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
     </row>
     <row r="5" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -1039,17 +1039,17 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
       <c r="K5" s="21"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
     </row>
     <row r="6" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="45"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1058,17 +1058,17 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
     </row>
     <row r="7" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -1079,17 +1079,17 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
       <c r="K7" s="21"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="44"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="44"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
     </row>
     <row r="8" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="45"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
@@ -1098,17 +1098,17 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
       <c r="K8" s="5"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
     </row>
     <row r="9" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="49" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -1119,17 +1119,17 @@
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
       <c r="K9" s="16"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
     </row>
     <row r="10" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="37"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1138,17 +1138,17 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
       <c r="K10" s="7"/>
       <c r="L10" s="6"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
     </row>
     <row r="11" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="49" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="15" t="s">
@@ -1159,17 +1159,17 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
       <c r="K11" s="16"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
     </row>
     <row r="12" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="37"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
@@ -1178,17 +1178,17 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
       <c r="K12" s="7"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
     </row>
     <row r="13" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="47" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1199,17 +1199,17 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
       <c r="K13" s="9"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
     </row>
     <row r="14" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="17" t="s">
         <v>11</v>
       </c>
@@ -1218,17 +1218,17 @@
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
       <c r="K14" s="18"/>
       <c r="L14" s="17"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
     </row>
     <row r="15" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="47" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1239,17 +1239,17 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
       <c r="K15" s="9"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="52"/>
     </row>
     <row r="16" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="17" t="s">
         <v>11</v>
       </c>
@@ -1258,17 +1258,17 @@
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
       <c r="K16" s="18"/>
       <c r="L16" s="17"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="52"/>
     </row>
     <row r="17" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="47" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1279,17 +1279,17 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
       <c r="K17" s="9"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="52"/>
     </row>
     <row r="18" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="40"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="17" t="s">
         <v>11</v>
       </c>
@@ -1298,17 +1298,17 @@
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
       <c r="K18" s="18"/>
       <c r="L18" s="17"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="48"/>
     </row>
     <row r="19" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="39" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="19" t="s">
@@ -1319,17 +1319,17 @@
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
       <c r="K19" s="20"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
     </row>
     <row r="20" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="34"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="10" t="s">
         <v>11</v>
       </c>
@@ -1338,17 +1338,17 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
       <c r="K20" s="11"/>
       <c r="L20" s="10"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
     </row>
     <row r="21" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="39" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="19" t="s">
@@ -1359,17 +1359,17 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
       <c r="K21" s="20"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
     </row>
     <row r="22" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="34"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="10" t="s">
         <v>11</v>
       </c>
@@ -1378,17 +1378,17 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
       <c r="K22" s="11"/>
       <c r="L22" s="10"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
     </row>
     <row r="23" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="39" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -1399,17 +1399,17 @@
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
       <c r="K23" s="20"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
     </row>
     <row r="24" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="34"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="10" t="s">
         <v>11</v>
       </c>
@@ -1418,36 +1418,33 @@
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
       <c r="K24" s="11"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="H5:H8"/>
-    <mergeCell ref="I5:I8"/>
-    <mergeCell ref="J5:J8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="H19:H24"/>
-    <mergeCell ref="I19:I24"/>
-    <mergeCell ref="J19:J24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="M19:M24"/>
+    <mergeCell ref="N19:N24"/>
+    <mergeCell ref="O19:O24"/>
+    <mergeCell ref="M9:M12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="O9:O12"/>
+    <mergeCell ref="M13:M18"/>
+    <mergeCell ref="N13:N18"/>
+    <mergeCell ref="O13:O18"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="M5:M8"/>
+    <mergeCell ref="N5:N8"/>
+    <mergeCell ref="O5:O8"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="N3:N4"/>
@@ -1464,22 +1461,25 @@
     <mergeCell ref="J13:J18"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="J3:J4"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="M19:M24"/>
-    <mergeCell ref="N19:N24"/>
-    <mergeCell ref="O19:O24"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="N9:N12"/>
-    <mergeCell ref="O9:O12"/>
-    <mergeCell ref="M13:M18"/>
-    <mergeCell ref="N13:N18"/>
-    <mergeCell ref="O13:O18"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="M5:M8"/>
-    <mergeCell ref="N5:N8"/>
-    <mergeCell ref="O5:O8"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="H19:H24"/>
+    <mergeCell ref="I19:I24"/>
+    <mergeCell ref="J19:J24"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="I5:I8"/>
+    <mergeCell ref="J5:J8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Lab 4 finalize commit
</commit_message>
<xml_diff>
--- a/assignments/Lab4_Tables.xlsx
+++ b/assignments/Lab4_Tables.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18165\Documents\R\Lab\biostatlab\assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BE50F0-C2AD-4433-97BC-C84986055965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD4607F-B879-4FD5-90B6-B8CB65A5EDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{441DAC2A-7180-4E9D-9169-FCB49694DB4E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,8 +33,60 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Nathan Ellermeier</author>
+  </authors>
+  <commentList>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{23E29125-EB2D-42C6-B94B-FBD9421D8B12}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Round to 3 decimals; report as a proportion</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{D4CA5CCE-5F63-4BB2-A765-A6E72DFC24AB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Round to 3 decimals</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{00C3C85E-9708-49F5-8579-137C00738453}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Round to 2 decimals</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Homogeneity Test</t>
   </si>
@@ -51,18 +103,12 @@
     <t>RD</t>
   </si>
   <si>
-    <t>CI</t>
-  </si>
-  <si>
     <t>Test Statistic</t>
   </si>
   <si>
     <t>p-value</t>
   </si>
   <si>
-    <t>IVW Pooled Estimator</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -111,20 +157,41 @@
     <t>Risk Ratio</t>
   </si>
   <si>
-    <t>Stratifying variable</t>
-  </si>
-  <si>
     <t>"exposure"</t>
   </si>
   <si>
     <t>Deaths ("outcome")</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>Strata</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>rural</t>
+  </si>
+  <si>
+    <t>magec</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>95% CI</t>
+  </si>
+  <si>
+    <t>Stdized Pooled Estimator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +255,27 @@
       <sz val="10"/>
       <color rgb="FF00B050"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -403,7 +491,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -488,46 +576,58 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -539,35 +639,63 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -891,597 +1019,638 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD95D8D6-7CA1-4C7B-995B-D96C674F8DDB}">
-  <dimension ref="A1:O24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD95D8D6-7CA1-4C7B-995B-D96C674F8DDB}">
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13:H18"/>
+      <selection pane="bottomRight" activeCell="O13" sqref="O13:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" customWidth="1"/>
-    <col min="9" max="9" width="11.77734375" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" customWidth="1"/>
-    <col min="11" max="12" width="13.44140625" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" style="59" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="59" customWidth="1"/>
+    <col min="3" max="3" width="15" style="59" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="59" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" style="59"/>
+    <col min="7" max="7" width="13.6640625" style="59" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" style="59" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" style="59" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" style="59" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" style="59" customWidth="1"/>
+    <col min="12" max="13" width="13.44140625" style="59" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" style="59" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="59" customWidth="1"/>
+    <col min="16" max="16" width="18" style="59" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="12"/>
+    <row r="1" spans="1:16" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="53" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="50"/>
+    </row>
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="54"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="47"/>
+      <c r="P2" s="25"/>
+    </row>
+    <row r="3" spans="1:16" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="56"/>
-      <c r="O2" s="25"/>
-    </row>
-    <row r="3" spans="1:15" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="O3" s="42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="58"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-    </row>
-    <row r="5" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="13"/>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="56"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+    </row>
+    <row r="5" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-    </row>
-    <row r="6" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="37"/>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="4"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+    </row>
+    <row r="6" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="61"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-    </row>
-    <row r="7" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="13" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="44"/>
+    </row>
+    <row r="7" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="61"/>
+      <c r="B7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="13"/>
+      <c r="C7" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-    </row>
-    <row r="8" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="37"/>
-      <c r="B8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="4"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+    </row>
+    <row r="8" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="62"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-    </row>
-    <row r="9" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="15"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
+    </row>
+    <row r="9" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="49"/>
-    </row>
-    <row r="10" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+    </row>
+    <row r="10" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="64"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
-    </row>
-    <row r="11" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="15"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+    </row>
+    <row r="11" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="64"/>
+      <c r="B11" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>8</v>
+      </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="51"/>
-    </row>
-    <row r="12" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="50"/>
-      <c r="B12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="6"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+    </row>
+    <row r="12" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="65"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-    </row>
-    <row r="13" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="8"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+    </row>
+    <row r="13" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
-    </row>
-    <row r="14" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="48"/>
-      <c r="B14" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="17"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+    </row>
+    <row r="14" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="67"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="17" t="s">
+        <v>9</v>
+      </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
-    </row>
-    <row r="15" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="8"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+    </row>
+    <row r="15" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="67"/>
+      <c r="B15" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
-    </row>
-    <row r="16" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="48"/>
-      <c r="B16" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="17"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+    </row>
+    <row r="16" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="67"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="17" t="s">
+        <v>9</v>
+      </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="52"/>
-    </row>
-    <row r="17" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="8"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+    </row>
+    <row r="17" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="67"/>
+      <c r="B17" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52"/>
-      <c r="O17" s="52"/>
-    </row>
-    <row r="18" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="48"/>
-      <c r="B18" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="17"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+    </row>
+    <row r="18" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="68"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="17" t="s">
+        <v>9</v>
+      </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48"/>
-      <c r="O18" s="48"/>
-    </row>
-    <row r="19" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="19"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+    </row>
+    <row r="19" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-    </row>
-    <row r="20" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="40"/>
-      <c r="B20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="10"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+    </row>
+    <row r="20" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="69"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
-    </row>
-    <row r="21" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="19"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+    </row>
+    <row r="21" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="69"/>
+      <c r="B21" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-    </row>
-    <row r="22" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="40"/>
-      <c r="B22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="10"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="33"/>
+    </row>
+    <row r="22" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="69"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-    </row>
-    <row r="23" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="19"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+    </row>
+    <row r="23" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="69"/>
+      <c r="B23" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-    </row>
-    <row r="24" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="40"/>
-      <c r="B24" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="10"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="33"/>
+    </row>
+    <row r="24" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="70"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40"/>
-      <c r="O24" s="40"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="M19:M24"/>
-    <mergeCell ref="N19:N24"/>
-    <mergeCell ref="O19:O24"/>
-    <mergeCell ref="M9:M12"/>
-    <mergeCell ref="N9:N12"/>
-    <mergeCell ref="O9:O12"/>
-    <mergeCell ref="M13:M18"/>
-    <mergeCell ref="N13:N18"/>
-    <mergeCell ref="O13:O18"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="M5:M8"/>
-    <mergeCell ref="N5:N8"/>
-    <mergeCell ref="O5:O8"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="J9:J12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="H13:H18"/>
-    <mergeCell ref="I13:I18"/>
-    <mergeCell ref="J13:J18"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="H19:H24"/>
-    <mergeCell ref="I19:I24"/>
-    <mergeCell ref="J19:J24"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="H5:H8"/>
-    <mergeCell ref="I5:I8"/>
-    <mergeCell ref="J5:J8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="H2:I2"/>
+  <mergeCells count="56">
+    <mergeCell ref="A5:A8"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="I2:J2"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="C3:C4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="I5:I8"/>
+    <mergeCell ref="J5:J8"/>
+    <mergeCell ref="K5:K8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="I19:I24"/>
+    <mergeCell ref="J19:J24"/>
+    <mergeCell ref="K19:K24"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="J9:J12"/>
+    <mergeCell ref="K9:K12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="I13:I18"/>
+    <mergeCell ref="J13:J18"/>
+    <mergeCell ref="K13:K18"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="N19:N24"/>
+    <mergeCell ref="O19:O24"/>
+    <mergeCell ref="P19:P24"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="O9:O12"/>
+    <mergeCell ref="P9:P12"/>
+    <mergeCell ref="N13:N18"/>
+    <mergeCell ref="O13:O18"/>
+    <mergeCell ref="P13:P18"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="N5:N8"/>
+    <mergeCell ref="O5:O8"/>
+    <mergeCell ref="P5:P8"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="L3:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>